<commit_message>
Update BOM with Ebay items numbers for critical parts
</commit_message>
<xml_diff>
--- a/BOM.xlsx
+++ b/BOM.xlsx
@@ -15,7 +15,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="165" uniqueCount="87">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="172" uniqueCount="97">
   <si>
     <t>Item</t>
   </si>
@@ -116,7 +116,7 @@
     <t>CONN, HDR, XH, 2 CKT</t>
   </si>
   <si>
-    <t>JST XH series knockoff</t>
+    <t>JST XH series knockoff*</t>
   </si>
   <si>
     <t>J2</t>
@@ -134,7 +134,7 @@
     <t>CONN, HDR, XH, 3 CKT</t>
   </si>
   <si>
-    <t>JST XH series knockoff. Remove center pin.</t>
+    <t>JST XH series knockoff*. Remove center pin.</t>
   </si>
   <si>
     <t>J6,J7</t>
@@ -146,6 +146,9 @@
     <t>KF7.62-2P</t>
   </si>
   <si>
+    <t>Ebay 231260624408</t>
+  </si>
+  <si>
     <t>K1</t>
   </si>
   <si>
@@ -158,6 +161,9 @@
     <t>8-1393239-5</t>
   </si>
   <si>
+    <t>Ebay 361282277725</t>
+  </si>
+  <si>
     <t>Product code RT314F05</t>
   </si>
   <si>
@@ -251,7 +257,10 @@
     <t>PSU, 5V, 1A, UNIV INPUT, ISOLATED</t>
   </si>
   <si>
-    <t>see picture, hole pattern must match main board</t>
+    <t>Ebay 351211320656</t>
+  </si>
+  <si>
+    <t>see picture, hole pattern must match main board.</t>
   </si>
   <si>
     <t>CONN, PLUG 3 POS</t>
@@ -276,6 +285,27 @@
   </si>
   <si>
     <t>Nylon Screw M2 6mm</t>
+  </si>
+  <si>
+    <t>*</t>
+  </si>
+  <si>
+    <t>A small kit of JST XH compatible</t>
+  </si>
+  <si>
+    <t>connectors is available on Ebay</t>
+  </si>
+  <si>
+    <t>under item 141292096528</t>
+  </si>
+  <si>
+    <t>This will have all of the headers</t>
+  </si>
+  <si>
+    <t>pins and housings you need</t>
+  </si>
+  <si>
+    <t>to build the project.</t>
   </si>
 </sst>
 </file>
@@ -372,10 +402,10 @@
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="A1:I32"/>
+  <dimension ref="A1:I40"/>
   <sheetViews>
     <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="I36" activeCellId="0" sqref="I36"/>
+      <selection pane="topLeft" activeCell="D41" activeCellId="0" sqref="D41"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.8"/>
@@ -386,7 +416,7 @@
     <col collapsed="false" hidden="false" max="4" min="4" style="0" width="29.030612244898"/>
     <col collapsed="false" hidden="false" max="5" min="5" style="0" width="45.4285714285714"/>
     <col collapsed="false" hidden="false" max="7" min="6" style="0" width="23.1989795918367"/>
-    <col collapsed="false" hidden="false" max="8" min="8" style="0" width="16.530612244898"/>
+    <col collapsed="false" hidden="false" max="8" min="8" style="0" width="19.0357142857143"/>
     <col collapsed="false" hidden="false" max="9" min="9" style="0" width="42.234693877551"/>
     <col collapsed="false" hidden="false" max="1025" min="10" style="0" width="11.5204081632653"/>
   </cols>
@@ -660,7 +690,7 @@
         <v>42</v>
       </c>
       <c r="H10" s="0" t="s">
-        <v>13</v>
+        <v>43</v>
       </c>
     </row>
     <row r="11" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -674,22 +704,22 @@
         <v>9</v>
       </c>
       <c r="D11" s="0" t="s">
-        <v>43</v>
+        <v>44</v>
       </c>
       <c r="E11" s="0" t="s">
-        <v>44</v>
+        <v>45</v>
       </c>
       <c r="F11" s="0" t="s">
-        <v>45</v>
+        <v>46</v>
       </c>
       <c r="G11" s="0" t="s">
-        <v>46</v>
+        <v>47</v>
       </c>
       <c r="H11" s="0" t="s">
-        <v>13</v>
+        <v>48</v>
       </c>
       <c r="I11" s="0" t="s">
-        <v>47</v>
+        <v>49</v>
       </c>
     </row>
     <row r="12" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -703,16 +733,16 @@
         <v>9</v>
       </c>
       <c r="D12" s="0" t="s">
-        <v>48</v>
+        <v>50</v>
       </c>
       <c r="E12" s="0" t="s">
-        <v>49</v>
+        <v>51</v>
       </c>
       <c r="F12" s="0" t="s">
-        <v>50</v>
+        <v>52</v>
       </c>
       <c r="G12" s="0" t="s">
-        <v>51</v>
+        <v>53</v>
       </c>
       <c r="H12" s="0" t="s">
         <v>13</v>
@@ -729,16 +759,16 @@
         <v>9</v>
       </c>
       <c r="D13" s="0" t="s">
-        <v>52</v>
+        <v>54</v>
       </c>
       <c r="E13" s="0" t="s">
-        <v>53</v>
+        <v>55</v>
       </c>
       <c r="F13" s="0" t="s">
-        <v>54</v>
+        <v>56</v>
       </c>
       <c r="G13" s="0" t="s">
-        <v>55</v>
+        <v>57</v>
       </c>
       <c r="H13" s="0" t="s">
         <v>19</v>
@@ -755,10 +785,10 @@
         <v>9</v>
       </c>
       <c r="D14" s="0" t="s">
-        <v>56</v>
+        <v>58</v>
       </c>
       <c r="E14" s="0" t="s">
-        <v>57</v>
+        <v>59</v>
       </c>
       <c r="F14" s="0" t="s">
         <v>12</v>
@@ -778,13 +808,13 @@
         <v>9</v>
       </c>
       <c r="D15" s="0" t="s">
-        <v>58</v>
+        <v>60</v>
       </c>
       <c r="E15" s="0" t="s">
-        <v>59</v>
+        <v>61</v>
       </c>
       <c r="F15" s="0" t="s">
-        <v>50</v>
+        <v>52</v>
       </c>
       <c r="H15" s="0" t="s">
         <v>13</v>
@@ -801,13 +831,13 @@
         <v>9</v>
       </c>
       <c r="D16" s="0" t="s">
-        <v>60</v>
+        <v>62</v>
       </c>
       <c r="E16" s="0" t="s">
-        <v>61</v>
+        <v>63</v>
       </c>
       <c r="F16" s="0" t="s">
-        <v>50</v>
+        <v>52</v>
       </c>
       <c r="H16" s="0" t="s">
         <v>13</v>
@@ -824,13 +854,13 @@
         <v>9</v>
       </c>
       <c r="D17" s="0" t="s">
-        <v>62</v>
+        <v>64</v>
       </c>
       <c r="E17" s="0" t="s">
-        <v>63</v>
+        <v>65</v>
       </c>
       <c r="F17" s="0" t="s">
-        <v>50</v>
+        <v>52</v>
       </c>
       <c r="H17" s="0" t="s">
         <v>13</v>
@@ -847,13 +877,13 @@
         <v>9</v>
       </c>
       <c r="D18" s="0" t="s">
-        <v>64</v>
+        <v>66</v>
       </c>
       <c r="E18" s="0" t="s">
-        <v>65</v>
+        <v>67</v>
       </c>
       <c r="F18" s="0" t="s">
-        <v>50</v>
+        <v>52</v>
       </c>
       <c r="H18" s="0" t="s">
         <v>13</v>
@@ -870,13 +900,13 @@
         <v>9</v>
       </c>
       <c r="D19" s="0" t="s">
-        <v>66</v>
+        <v>68</v>
       </c>
       <c r="E19" s="0" t="s">
-        <v>67</v>
+        <v>69</v>
       </c>
       <c r="F19" s="0" t="s">
-        <v>50</v>
+        <v>52</v>
       </c>
       <c r="H19" s="0" t="s">
         <v>13</v>
@@ -896,16 +926,16 @@
         <v>9</v>
       </c>
       <c r="D20" s="0" t="s">
-        <v>68</v>
+        <v>70</v>
       </c>
       <c r="E20" s="0" t="s">
-        <v>69</v>
+        <v>71</v>
       </c>
       <c r="F20" s="0" t="s">
-        <v>50</v>
+        <v>52</v>
       </c>
       <c r="G20" s="0" t="s">
-        <v>70</v>
+        <v>72</v>
       </c>
       <c r="H20" s="0" t="s">
         <v>13</v>
@@ -922,16 +952,16 @@
         <v>9</v>
       </c>
       <c r="D21" s="0" t="s">
-        <v>71</v>
+        <v>73</v>
       </c>
       <c r="E21" s="0" t="s">
-        <v>72</v>
+        <v>74</v>
       </c>
       <c r="F21" s="0" t="s">
-        <v>73</v>
+        <v>75</v>
       </c>
       <c r="G21" s="0" t="s">
-        <v>74</v>
+        <v>76</v>
       </c>
       <c r="H21" s="0" t="s">
         <v>19</v>
@@ -939,7 +969,7 @@
     </row>
     <row r="23" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="D23" s="0" t="s">
-        <v>75</v>
+        <v>77</v>
       </c>
     </row>
     <row r="25" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -953,19 +983,19 @@
         <v>9</v>
       </c>
       <c r="D25" s="0" t="s">
-        <v>76</v>
+        <v>78</v>
       </c>
       <c r="E25" s="0" t="s">
-        <v>77</v>
+        <v>79</v>
       </c>
       <c r="F25" s="0" t="s">
-        <v>50</v>
+        <v>52</v>
       </c>
       <c r="H25" s="0" t="s">
-        <v>13</v>
+        <v>80</v>
       </c>
       <c r="I25" s="0" t="s">
-        <v>78</v>
+        <v>81</v>
       </c>
     </row>
     <row r="26" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -979,10 +1009,10 @@
         <v>9</v>
       </c>
       <c r="E26" s="0" t="s">
-        <v>79</v>
+        <v>82</v>
       </c>
       <c r="F26" s="0" t="s">
-        <v>50</v>
+        <v>52</v>
       </c>
       <c r="H26" s="0" t="s">
         <v>13</v>
@@ -1002,10 +1032,10 @@
         <v>9</v>
       </c>
       <c r="E27" s="0" t="s">
-        <v>80</v>
+        <v>83</v>
       </c>
       <c r="F27" s="0" t="s">
-        <v>50</v>
+        <v>52</v>
       </c>
       <c r="H27" s="0" t="s">
         <v>13</v>
@@ -1025,10 +1055,10 @@
         <v>9</v>
       </c>
       <c r="E28" s="0" t="s">
-        <v>81</v>
+        <v>84</v>
       </c>
       <c r="F28" s="0" t="s">
-        <v>50</v>
+        <v>52</v>
       </c>
       <c r="H28" s="0" t="s">
         <v>13</v>
@@ -1045,13 +1075,13 @@
         <v>0.001</v>
       </c>
       <c r="C29" s="0" t="s">
-        <v>82</v>
+        <v>85</v>
       </c>
       <c r="E29" s="0" t="s">
-        <v>83</v>
+        <v>86</v>
       </c>
       <c r="F29" s="0" t="s">
-        <v>50</v>
+        <v>52</v>
       </c>
       <c r="H29" s="0" t="s">
         <v>13</v>
@@ -1068,10 +1098,10 @@
         <v>9</v>
       </c>
       <c r="E30" s="0" t="s">
-        <v>84</v>
+        <v>87</v>
       </c>
       <c r="F30" s="0" t="s">
-        <v>50</v>
+        <v>52</v>
       </c>
       <c r="H30" s="0" t="s">
         <v>13</v>
@@ -1088,10 +1118,10 @@
         <v>9</v>
       </c>
       <c r="E31" s="0" t="s">
-        <v>85</v>
+        <v>88</v>
       </c>
       <c r="F31" s="0" t="s">
-        <v>50</v>
+        <v>52</v>
       </c>
       <c r="H31" s="0" t="s">
         <v>13</v>
@@ -1108,13 +1138,46 @@
         <v>9</v>
       </c>
       <c r="E32" s="0" t="s">
-        <v>86</v>
+        <v>89</v>
       </c>
       <c r="F32" s="0" t="s">
-        <v>50</v>
+        <v>52</v>
       </c>
       <c r="H32" s="0" t="s">
         <v>13</v>
+      </c>
+    </row>
+    <row r="35" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="B35" s="0" t="s">
+        <v>90</v>
+      </c>
+      <c r="D35" s="0" t="s">
+        <v>91</v>
+      </c>
+    </row>
+    <row r="36" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="D36" s="0" t="s">
+        <v>92</v>
+      </c>
+    </row>
+    <row r="37" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="D37" s="0" t="s">
+        <v>93</v>
+      </c>
+    </row>
+    <row r="38" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="D38" s="0" t="s">
+        <v>94</v>
+      </c>
+    </row>
+    <row r="39" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="D39" s="0" t="s">
+        <v>95</v>
+      </c>
+    </row>
+    <row r="40" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="D40" s="0" t="s">
+        <v>96</v>
       </c>
     </row>
   </sheetData>

</xml_diff>